<commit_message>
General trace information mechanisms abnd ODM-specific trace information
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes.xlsx
+++ b/apps/delphes/runtime/configuration_delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5649693-0FA2-4E46-98FD-CDD4BDA9A8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927DE33E-BDA7-4F52-BD5C-D6607836DBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="173">
   <si>
     <t>response_format_type</t>
   </si>
@@ -631,6 +631,9 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>trace_rules</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2165,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2560B-2446-422E-A0A3-EC959CE749E5}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,6 +2194,14 @@
       </c>
       <c r="B2" s="12" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cache_ok with ideal results
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes.xlsx
+++ b/apps/delphes/runtime/configuration_delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F3A782-693F-46A4-A912-024D041D0BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF455E48-60BD-467B-9D0C-841861AFA4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="12" r:id="rId1"/>
@@ -1054,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1426,9 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1787,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1860,7 @@
         <v>160</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Add all rules that were missing
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes.xlsx
+++ b/apps/delphes/runtime/configuration_delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF455E48-60BD-467B-9D0C-841861AFA4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C770F7B8-429A-487C-8D52-85F064FB7852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11010" yWindow="0" windowWidth="14400" windowHeight="15480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="12" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="definitions" sheetId="7" r:id="rId5"/>
     <sheet name="intentions" sheetId="2" r:id="rId6"/>
     <sheet name="odm" sheetId="15" r:id="rId7"/>
-    <sheet name="dmoe" sheetId="16" r:id="rId8"/>
+    <sheet name="drools" sheetId="16" r:id="rId8"/>
     <sheet name="email_configuration" sheetId="13" r:id="rId9"/>
     <sheet name="email_templates" sheetId="11" r:id="rId10"/>
     <sheet name="tests" sheetId="9" r:id="rId11"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="182">
   <si>
     <t>response_format_type</t>
   </si>
@@ -529,9 +529,6 @@
     <t>type_str</t>
   </si>
   <si>
-    <t>21/05/2025</t>
-  </si>
-  <si>
     <t>Aujourd'hui est le {date_demande} (JJ/MM/AAAA).
 Vous êtes un agent en charge d'analyser des demandes en rapport avec les procédures d'Asile ou de Séjour envoyées par des demandeurs étrangers à une Préfecture de département.</t>
   </si>
@@ -624,15 +621,6 @@
     <t>http://localhost:9060/DecisionService/rest/delphes/case_handling_decision</t>
   </si>
   <si>
-    <t>Either odm, dmoe or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
-  </si>
-  <si>
-    <t>dmoe_param</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>trace_rules</t>
   </si>
   <si>
@@ -646,6 +634,40 @@
   </si>
   <si>
     <t>api-a-renouveler</t>
+  </si>
+  <si>
+    <t>runtime_directory</t>
+  </si>
+  <si>
+    <t>apps/delphes/runtime</t>
+  </si>
+  <si>
+    <t>The directory where various app-specific runtime artefacts are stored, in particular the caching of text analysis. It is relative to the directory from where the app is run</t>
+  </si>
+  <si>
+    <t>sauf-conduits</t>
+  </si>
+  <si>
+    <t>Votre demande de sauf-conduit</t>
+  </si>
+  <si>
+    <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
+  </si>
+  <si>
+    <t>drools_param</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+En réponse à votre demande, je vous invite à nous adresser une copie des éléments suivants :
+- l’acte de décès traduit
+- votre acte de naissance
+- la date des funérailles
+- votre carte de séjour
+- d'un justificatif de domicile de moins de 6 mois en indiquant en objet URGENT DEMANDE DE SAUF CONDUIT.
+En espérant vous avoir apporté les éléments souhaités,</t>
+  </si>
+  <si>
+    <t>15/9/2024</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,21 +1091,32 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>167</v>
+      <c r="B3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1372,17 +1405,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="151.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1398,23 +1431,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1426,7 +1470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1456,7 +1502,7 @@
         <v>123</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>135</v>
@@ -1485,10 +1531,10 @@
         <v>136</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="8" t="b">
         <v>1</v>
@@ -1520,7 +1566,7 @@
         <v>128</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="8" t="b">
         <v>1</v>
@@ -1549,10 +1595,10 @@
         <v>116</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F4" s="8" t="b">
         <v>1</v>
@@ -1581,10 +1627,10 @@
         <v>114</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="8" t="b">
         <v>1</v>
@@ -1613,10 +1659,10 @@
         <v>120</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F6" s="8" t="b">
         <v>1</v>
@@ -1645,10 +1691,10 @@
         <v>119</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" s="8" t="b">
         <v>1</v>
@@ -1680,7 +1726,7 @@
         <v>127</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="8" t="b">
         <v>1</v>
@@ -1712,7 +1758,7 @@
         <v>127</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" s="7" t="b">
         <v>0</v>
@@ -1730,19 +1776,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F10" s="8" t="b">
         <v>1</v>
@@ -1751,7 +1797,7 @@
         <v>73</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>133</v>
@@ -1785,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,25 +1897,25 @@
         <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -2232,15 +2278,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B3" s="7" t="b">
         <v>1</v>
@@ -2259,7 +2305,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,10 +2324,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2317,25 +2363,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>117</v>
@@ -2344,25 +2390,25 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>

</xml_diff>

<commit_message>
Finish implementation of all rules (same level as legacy POC) + Parameterize Excel file + update READMR & TODO
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes.xlsx
+++ b/apps/delphes/runtime/configuration_delphes.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C770F7B8-429A-487C-8D52-85F064FB7852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A19F9B4-48FA-42C8-9D65-C6DE3DCB6C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11010" yWindow="0" windowWidth="14400" windowHeight="15480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="12" r:id="rId1"/>
-    <sheet name="backend" sheetId="14" r:id="rId2"/>
-    <sheet name="case_fields" sheetId="10" r:id="rId3"/>
-    <sheet name="text_analysis" sheetId="1" r:id="rId4"/>
-    <sheet name="definitions" sheetId="7" r:id="rId5"/>
-    <sheet name="intentions" sheetId="2" r:id="rId6"/>
-    <sheet name="odm" sheetId="15" r:id="rId7"/>
-    <sheet name="drools" sheetId="16" r:id="rId8"/>
-    <sheet name="email_configuration" sheetId="13" r:id="rId9"/>
-    <sheet name="email_templates" sheetId="11" r:id="rId10"/>
-    <sheet name="tests" sheetId="9" r:id="rId11"/>
-    <sheet name="tests long" sheetId="4" r:id="rId12"/>
-    <sheet name="tests short" sheetId="8" r:id="rId13"/>
+    <sheet name="frontend" sheetId="17" r:id="rId2"/>
+    <sheet name="backend" sheetId="14" r:id="rId3"/>
+    <sheet name="case_fields" sheetId="10" r:id="rId4"/>
+    <sheet name="text_analysis" sheetId="1" r:id="rId5"/>
+    <sheet name="definitions" sheetId="7" r:id="rId6"/>
+    <sheet name="intentions" sheetId="2" r:id="rId7"/>
+    <sheet name="odm" sheetId="15" r:id="rId8"/>
+    <sheet name="drools" sheetId="16" r:id="rId9"/>
+    <sheet name="email_configuration" sheetId="13" r:id="rId10"/>
+    <sheet name="email_templates" sheetId="11" r:id="rId11"/>
+    <sheet name="tests" sheetId="9" r:id="rId12"/>
+    <sheet name="tests long" sheetId="4" r:id="rId13"/>
+    <sheet name="tests short" sheetId="8" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="188">
   <si>
     <t>response_format_type</t>
   </si>
@@ -651,9 +652,6 @@
     <t>Votre demande de sauf-conduit</t>
   </si>
   <si>
-    <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
-  </si>
-  <si>
     <t>drools_param</t>
   </si>
   <si>
@@ -668,6 +666,29 @@
   </si>
   <si>
     <t>15/9/2024</t>
+  </si>
+  <si>
+    <t>connection_to_api</t>
+  </si>
+  <si>
+    <t>direct</t>
+  </si>
+  <si>
+    <t>http_connection_url</t>
+  </si>
+  <si>
+    <t>http://localhost:8002</t>
+  </si>
+  <si>
+    <t>For instance http://localhost:8002 if launched: fastapi dev .\launcher_fastapi.py --port 8002</t>
+  </si>
+  <si>
+    <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython
+Currently, only odm works</t>
+  </si>
+  <si>
+    <t>Either http or direct
+Currently only direct works</t>
   </si>
 </sst>
 </file>
@@ -1073,6 +1094,96 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="5">
+        <v>587</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D837CF12-5C63-4697-8041-1E2C28E86DD4}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{4DA7E683-0DA1-40B9-9F1D-EC7A05076326}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1116,7 +1227,7 @@
         <v>177</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1124,7 +1235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC612E36-7152-48D2-8E3D-E1FAD4D4F885}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1169,7 +1280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A251C2B-C886-421E-8876-0F07524CBA66}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -1358,7 +1469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9702681-D1BC-443E-80AD-3DFE6E5250FB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1404,11 +1515,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,6 +1540,68 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{178CE984-2701-4FB0-A6D8-D84336AB1260}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="151.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>173</v>
@@ -1440,15 +1613,15 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>178</v>
+      <c r="C3" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1466,11 +1639,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1531,7 +1704,7 @@
         <v>136</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>145</v>
@@ -1827,12 +2000,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,7 +2098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1992,7 +2165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -2254,12 +2427,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2560B-2446-422E-A0A3-EC959CE749E5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,7 +2473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67526D7-3946-41B7-9C99-93B1591CF2D0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2324,103 +2497,13 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="5">
-        <v>587</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D837CF12-5C63-4697-8041-1E2C28E86DD4}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{4DA7E683-0DA1-40B9-9F1D-EC7A05076326}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalize ODM decision service + README almost finalized
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes.xlsx
+++ b/apps/delphes/runtime/configuration_delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A19F9B4-48FA-42C8-9D65-C6DE3DCB6C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3FA946-762B-4F94-A4C0-ABAF473FD742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="12" r:id="rId1"/>
@@ -671,9 +671,6 @@
     <t>connection_to_api</t>
   </si>
   <si>
-    <t>direct</t>
-  </si>
-  <si>
     <t>http_connection_url</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
   </si>
   <si>
     <t>For instance http://localhost:8002 if launched: fastapi dev .\launcher_fastapi.py --port 8002</t>
+  </si>
+  <si>
+    <t>http</t>
   </si>
   <si>
     <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1545,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>187</v>
@@ -1553,13 +1553,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1580,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>